<commit_message>
Update DateBase/orders/International Ever Green_2025-11-21.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2025-11-21.xlsx
+++ b/DateBase/orders/International Ever Green_2025-11-21.xlsx
@@ -949,6 +949,9 @@
       <c r="C61" t="str">
         <v>7_翠绿洋桔梗_Dark Green Lisianthus_Eustoma grandiflorum (Raf.) Shinners_800/600g</v>
       </c>
+      <c r="F61" t="str">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -1010,7 +1013,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>0151585158168103152060301010151202093017201510101510302015202020101020335555355855551055555120</v>
+        <v>0151585158168103152060301010151202093017201510101510302015202020101020335555355855551055555125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>